<commit_message>
excel coded: fix namespace + pivot table test
</commit_message>
<xml_diff>
--- a/CodedExcelDemo/codedExcel3.xlsx
+++ b/CodedExcelDemo/codedExcel3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viorel.groza\OneDrive - UiPath\Documents\myUiPath\CodedDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\codedautomations-samples\CodedExcelDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FD0FAE-FBF8-40C4-A36F-8E9CE762D143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E4402-FEB3-45C5-AF89-6BD6FDE000A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26520" yWindow="4896" windowWidth="19992" windowHeight="7380" firstSheet="8" activeTab="10" xr2:uid="{3F37A5E2-7F99-4D3A-B4DF-927DEFC364F7}"/>
+    <workbookView xWindow="-26868" yWindow="4548" windowWidth="19992" windowHeight="7380" activeTab="3" xr2:uid="{3F37A5E2-7F99-4D3A-B4DF-927DEFC364F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -34,8 +34,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId12"/>
-    <pivotCache cacheId="11" r:id="rId13"/>
+    <pivotCache cacheId="16" r:id="rId12"/>
+    <pivotCache cacheId="17" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="38">
   <si>
     <t>aa1</t>
   </si>
@@ -206,13 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +528,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DFF7F570-1D4F-4F89-B7F5-39DFF0D30FFB}" name="myNewPT" cacheId="11" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DFF7F570-1D4F-4F89-B7F5-39DFF0D30FFB}" name="myNewPT" cacheId="17" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0" includeNewItemsInFilter="1">
@@ -659,7 +658,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A3789D0-CD67-4AE4-B06C-2C2BB609C830}" name="newPivot" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A3789D0-CD67-4AE4-B06C-2C2BB609C830}" name="newPivot" cacheId="16" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A1:F6" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" multipleItemSelectionAllowed="1" showAll="0" includeNewItemsInFilter="1">
@@ -1101,10 +1100,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F674AB-6E6B-4E2B-848F-6FDCF8F016B3}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B34"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1493,11 +1492,301 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1775,7 +2064,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1841,15 +2130,13 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
     </row>
@@ -1857,15 +2144,13 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
     </row>
@@ -1873,19 +2158,19 @@
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>6</v>
       </c>
     </row>
@@ -2071,7 +2356,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3732,15 +4017,10 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
     </row>
@@ -3748,15 +4028,10 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
     </row>
@@ -3764,15 +4039,10 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="H7">
         <v>3</v>
       </c>
     </row>
@@ -3780,15 +4050,10 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="H8">
         <v>3</v>
       </c>
     </row>
@@ -3796,15 +4061,10 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3">
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="H9">
         <v>3</v>
       </c>
     </row>
@@ -3812,15 +4072,10 @@
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
@@ -3828,25 +4083,25 @@
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>16</v>
       </c>
     </row>

</xml_diff>